<commit_message>
Edited Scheduler and created Subsystem Address
Added more methods to Scheduler class and created SubsystemAddress to hold addresses of each subsystem
</commit_message>
<xml_diff>
--- a/Request formats.xlsx
+++ b/Request formats.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>ORG type</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>bytes</t>
+  </si>
+  <si>
+    <t>ElevatorInputPacket</t>
   </si>
 </sst>
 </file>
@@ -533,7 +536,7 @@
         <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>